<commit_message>
+Worked on downloaded pdf path
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_5_a\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF6D00A-903A-451F-B98A-3BEF8A323A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E1D1CE-353A-40AF-A186-A41096F484FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>Exception message if the invoice details cannot be updated</t>
+  </si>
+  <si>
+    <t>PdfPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_5_a\Data\Input\</t>
   </si>
 </sst>
 </file>
@@ -677,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1781,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2097,7 +2103,14 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>